<commit_message>
correciones en carga de archivo excel
</commit_message>
<xml_diff>
--- a/src/views/paginas/Finanzas/archivos/upload/Clientesporlotes.xlsx
+++ b/src/views/paginas/Finanzas/archivos/upload/Clientesporlotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D7B0A5-31D7-4E02-838F-7B5342B641F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BF74F1-85B5-4FB0-9BDD-02D36ED482CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{112C8200-8E67-43F8-B4BF-AD833F782847}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>DNI</t>
   </si>
@@ -51,76 +51,82 @@
     <t>AnticipoFinanciero</t>
   </si>
   <si>
-    <t>Miranda, Adrian</t>
-  </si>
-  <si>
-    <t>Palacios, Luis</t>
-  </si>
-  <si>
-    <t>Maximiliano, Perez Alvares</t>
-  </si>
-  <si>
-    <t>Molina, Juan Carlos</t>
-  </si>
-  <si>
-    <t>Carratala, Cristian</t>
-  </si>
-  <si>
-    <t>Gil, Dario</t>
-  </si>
-  <si>
-    <t>Franco Del Piccolo</t>
-  </si>
-  <si>
-    <t>Alvarez, Fernando</t>
-  </si>
-  <si>
-    <t>Carrizo, Carolina</t>
-  </si>
-  <si>
-    <t>M. Correa y Estefania</t>
-  </si>
-  <si>
-    <t>Jorge Luis Yarzabal</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A12</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
-    <t>A8</t>
-  </si>
-  <si>
-    <t>A9</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
-    <t>A11</t>
-  </si>
-  <si>
-    <t>A13</t>
+    <t>ServicioDomiciliario</t>
+  </si>
+  <si>
+    <t>Bordon Daniela Romina</t>
+  </si>
+  <si>
+    <t>Urbieta Pedro Adolfo</t>
+  </si>
+  <si>
+    <t>Pelizza Marta Beatriz</t>
+  </si>
+  <si>
+    <t>Morales Andres Eduardo</t>
+  </si>
+  <si>
+    <t>Soria Luis Fernando</t>
+  </si>
+  <si>
+    <t>Gonzalez Eduardo Raimundo</t>
+  </si>
+  <si>
+    <t>Fattore Silvia</t>
+  </si>
+  <si>
+    <t>Herrera Dominguez Gilberto Carlos Emanuel</t>
+  </si>
+  <si>
+    <t>Agüero Claudio Esteban</t>
+  </si>
+  <si>
+    <t>Chaile Manuel Jesus</t>
+  </si>
+  <si>
+    <t>Bordalecu Maria Cristina</t>
+  </si>
+  <si>
+    <t>Puebla Nilda</t>
+  </si>
+  <si>
+    <t>Robledo Morales Gonzalo</t>
+  </si>
+  <si>
+    <t>Peñaloza Irma</t>
+  </si>
+  <si>
+    <t>Chaile Ramon Eduardo</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -128,9 +134,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,16 +145,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -161,36 +173,23 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FF92D050"/>
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF00B050"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -221,22 +220,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -244,57 +279,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF5050"/>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -306,16 +290,17 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@"/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
+          <fgColor rgb="FF00B050"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -326,7 +311,9 @@
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
-        <top/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -345,18 +332,85 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@"/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
+          <fgColor rgb="FF00B050"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -368,9 +422,7 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
@@ -389,17 +441,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}" name="Tabla1" displayName="Tabla1" ref="A1:H14" totalsRowShown="0">
-  <autoFilter ref="A1:H14" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}" name="Tabla1" displayName="Tabla1" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8E528A00-2794-476A-936B-E771A6D11F9F}" name="Nombre" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{0DE29ACD-DE4C-41BD-822D-FB2DE07BF89E}" name="DNI"/>
     <tableColumn id="4" xr3:uid="{A0E1F818-7EE2-421B-8AC2-193492055A92}" name="Telefono"/>
     <tableColumn id="5" xr3:uid="{9B876E5B-EBB3-4AB1-B206-B748A7AC4118}" name="Correo"/>
     <tableColumn id="6" xr3:uid="{6A96E5A5-A177-40B4-BFFD-2C896C2F2D8A}" name="MznaYLote" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{0A49A181-EA67-4FBE-95AD-8BC71FF197E1}" name="CuotasXCobrar"/>
-    <tableColumn id="9" xr3:uid="{611BB5E5-4545-4552-9873-DF465C9A669D}" name="MontoCuota" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{788F0D6E-A424-47BD-8F41-9E8C652FD76D}" name="AnticipoFinanciero"/>
+    <tableColumn id="9" xr3:uid="{611BB5E5-4545-4552-9873-DF465C9A669D}" name="MontoCuota" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{788F0D6E-A424-47BD-8F41-9E8C652FD76D}" name="AnticipoFinanciero" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{2CD4C72B-C7B2-4150-9C79-2D427D4C8E2A}" name="ServicioDomiciliario"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -703,10 +756,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFAE7C3-B067-4F00-A6C5-90768CB2152A}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,9 +772,10 @@
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -746,195 +800,301 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="93" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H2" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I2">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H3" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I3">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H4" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I4">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H5" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I5">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H6" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I6">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H7" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I7">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H8" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I8">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H9" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I9">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H10" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I10">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H11" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I11">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="69.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="E12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H12" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I12">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H13" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I13">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="69.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="E14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H14" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I14">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="139.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="E15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H15" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I15">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="93" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="93" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="93" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="93" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="93" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="93" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="116.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="93" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" s="4">
-        <v>1700</v>
+      <c r="E16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16" s="7">
+        <v>3172.64</v>
+      </c>
+      <c r="H16" s="8">
+        <v>17630.849999999999</v>
+      </c>
+      <c r="I16">
+        <v>7500</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
-      <formula>1700</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>